<commit_message>
Refactor and enhance account creation process
Added TempMailOrg class for temporary email generation and integrated it with the account creation functions. Improved UI/UX in kag_tools.py, including theming, layout adjustments, and RTL support. Refined logic in account_creator.py with better error handling, email overriding, and script organization.
</commit_message>
<xml_diff>
--- a/data/accounts.xlsx
+++ b/data/accounts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,10 +740,554 @@
           <t>male</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>2025-04-19 19:25:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sarah Garcia</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sarah.brown81@hotmail.com</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Pass3292</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4 December 1989</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:53:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sarah Garcia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sarah.brown81@hotmail.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Pass3292</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4 December 1989</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:53:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sarah Jones</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sarah.johnson72@outlook.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Pass3942</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>28 July 1992</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:54:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sarah Jones</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sarah.johnson72@outlook.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Pass3942</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>28 July 1992</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:54:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>James Brown</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>james.johnson24@protonmail.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Pass4590</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>27 October 1992</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:54:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>James Brown</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>james.johnson24@protonmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Pass4590</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>27 October 1992</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:54:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>James Jones</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>james.williams45@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Pass2039</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>8 September 1985</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:57:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>James Jones</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>james.williams45@gmail.com</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Pass2039</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>8 September 1985</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-04-19 20:57:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>john.johnson6@protonmail.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Pass2867</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>22 March 1995</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:07:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>john.johnson6@protonmail.com</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Pass2867</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>22 March 1995</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:07:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Emma Brown</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Loading</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Pass5452</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3 December 1987</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:12:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Emma Brown</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Loading</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Pass5452</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3 December 1987</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:12:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>John Williams</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Loading</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Pass8711</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>4 October 1990</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:12:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Emma Jones</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>wasaro6972@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Pass6375</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>20 September 1990</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:14:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Emma Jones</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>wasaro6972@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Pass6375</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>20 September 1990</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:14:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>John Garcia</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>nilono4638@f5url.com</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Pass3288</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>20 March 1988</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>John Garcia</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>nilono4638@f5url.com</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Pass3288</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>20 March 1988</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:15:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor temporary email retrieval and improve UI layout
Moved temp email logic to `TempMailOrg` for better reusability. Enhanced GUI layout with tighter spacing, RTL support, and icons for clarity. Streamlined random data handling and entry validation logic in the form generator.
</commit_message>
<xml_diff>
--- a/data/accounts.xlsx
+++ b/data/accounts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1284,10 +1284,490 @@
           <t>male</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>2025-04-19 21:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Emma Williams</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>yotixog229@bauscn.com</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Pass1231</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>28 April 1982</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:47:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Emma Williams</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>yotixog229@bauscn.com</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Pass1231</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>28 April 1982</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:47:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>woroko1536@f5url.com</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Pass9639</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>21 October 1984</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:59:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>woroko1536@f5url.com</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Pass9639</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>21 October 1984</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:59:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>poyef47285@cotigz.com</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Pass9639</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>21 October 1984</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:59:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>poyef47285@cotigz.com</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Pass9639</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>21 October 1984</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-04-19 21:59:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>James Williams</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>james.jones47@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Pass3195</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>12 June 1989</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-04-19 22:02:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Olivia Johnson</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>nigip97395@linxues.com</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Pass5396</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>17 September 1981</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-04-19 22:03:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Olivia Johnson</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>nigip97395@linxues.com</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Pass5396</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>17 September 1981</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-04-19 22:03:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>John Brown</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mosakar418@f5url.com</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Pass4832</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>19 February 1989</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:32:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>John Brown</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mosakar418@f5url.com</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Pass4832</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>19 February 1989</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:32:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>James Smith</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>jawidam390@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Pass1348</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7 September 1999</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:36:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>James Smith</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>jawidam390@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Pass1348</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>7 September 1999</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:36:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>James Smith</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>wimatog888@cxnlab.com</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Pass1348</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>7 September 1999</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:37:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>James Smith</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>wimatog888@cxnlab.com</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Pass1348</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>7 September 1999</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:37:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor temp email logic and switch from email to username
Updated temporary email handling to use 1secmail instead of temp-mail.org, adding support for verification code retrieval. Changed the system to prioritize 'username' over 'email', reflecting this in data generators, account creator logic, and GUI fields. Also added new dependencies (aiohttp, pydantic, requests) for enhanced functionality.
</commit_message>
<xml_diff>
--- a/data/accounts.xlsx
+++ b/data/accounts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1764,10 +1764,234 @@
           <t>male</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
           <t>2025-04-19 23:37:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Michael Smith</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>bapije3413@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Pass8934</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>15 September 1983</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:46:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Michael Smith</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>bapije3413@agiuse.com</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Pass8934</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>15 September 1983</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-04-19 23:46:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>John Garcia</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>johngarcia52@maildrop.cc</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Pass7741</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>20 December 1989</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-04-20 00:49:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>John Garcia</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>johngarcia52@maildrop.cc</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Pass7741</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>20 December 1989</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-04-20 00:49:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Emma Smith</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>emmasmith62@maildrop.cc</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Pass6692</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>20 June 1991</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-04-20 00:50:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Sarah Brown</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>oceubme753@1secmail.website</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Pass9123</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>23 April 1998</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-04-20 01:18:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Sarah Brown</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>oceubme753@1secmail.website</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Pass9123</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>23 April 1998</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>female</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-04-20 01:18:13</t>
         </is>
       </c>
     </row>

</xml_diff>